<commit_message>
Fixed negative for export prices on SAF
Export ACT COST of SAF were positive, have changed this to negative.
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_SUP_SAF.xlsx
+++ b/SubRes_TMPL/SubRES_SUP_SAF.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C559A1F-FE44-4C21-825D-F8148ACB4CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2FBB90-0538-4385-87A1-20E59908697D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DC2DED06-3C4E-4822-B6CB-2383E5736C95}"/>
+    <workbookView xWindow="9135" yWindow="3780" windowWidth="16440" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9480" yWindow="4125" windowWidth="16440" windowHeight="11055" xr2:uid="{DC2DED06-3C4E-4822-B6CB-2383E5736C95}"/>
   </bookViews>
   <sheets>
     <sheet name="Aviation Synfuel" sheetId="5" r:id="rId1"/>
@@ -3985,8 +3985,8 @@
   </sheetPr>
   <dimension ref="A11:V238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N72" sqref="N72:Q72"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
@@ -4981,20 +4981,20 @@
         <v>204</v>
       </c>
       <c r="D81" s="8">
-        <f>D70*(1+D71)</f>
-        <v>376.15110464174512</v>
+        <f>-D70*(1+D71)</f>
+        <v>-376.15110464174512</v>
       </c>
       <c r="E81" s="8">
-        <f>E70*(1+E71)</f>
-        <v>346.83700531185411</v>
+        <f>-E70*(1+E71)</f>
+        <v>-346.83700531185411</v>
       </c>
       <c r="G81" s="8">
-        <f>G70*(1+G71)</f>
-        <v>436.50366208563838</v>
+        <f>-G70*(1+G71)</f>
+        <v>-436.50366208563838</v>
       </c>
       <c r="I81" s="8">
-        <f>I70*(1+I71)</f>
-        <v>436.50366208563838</v>
+        <f>-I70*(1+I71)</f>
+        <v>-436.50366208563838</v>
       </c>
       <c r="N81" s="91"/>
     </row>

</xml_diff>